<commit_message>
Functional Match values validation
</commit_message>
<xml_diff>
--- a/test/input/FullValuesAndComments.xlsx
+++ b/test/input/FullValuesAndComments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
   <si>
     <t>Input Value</t>
   </si>
@@ -105,6 +105,12 @@
     <t>Short Title</t>
   </si>
   <si>
+    <t>Functional Match 1</t>
+  </si>
+  <si>
+    <t>Functional Match 2</t>
+  </si>
+  <si>
     <t>Founder</t>
   </si>
   <si>
@@ -177,6 +183,15 @@
     <t>ExTi1</t>
   </si>
   <si>
+    <t>CAO</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>COO</t>
+  </si>
+  <si>
     <t>lala</t>
   </si>
   <si>
@@ -196,6 +211,12 @@
   </si>
   <si>
     <t>C4</t>
+  </si>
+  <si>
+    <t>fm1com</t>
+  </si>
+  <si>
+    <t>fm2com</t>
   </si>
   <si>
     <t>C5</t>
@@ -455,12 +476,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4392156862745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5529411764706"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.556862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -631,23 +652,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD14"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="Q6" activeCellId="0" pane="topLeft" sqref="Q6"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="G4" activeCellId="0" pane="topLeft" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.57254901960784"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4117647058824"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.9254901960784"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4392156862745"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.90980392156863"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.9254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.3843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.5921568627451"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="8.3843137254902"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.4313725490196"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.4588235294118"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.3843137254902"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.92941176470588"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.3843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -658,20 +679,20 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
@@ -681,13 +702,15 @@
       <c r="W1" s="9"/>
       <c r="X1" s="9"/>
       <c r="Y1" s="9"/>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
       <c r="AC1" s="9"/>
       <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="B2" s="9"/>
@@ -695,22 +718,22 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
-      <c r="L2" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
@@ -725,6 +748,8 @@
       <c r="AB2" s="9"/>
       <c r="AC2" s="9"/>
       <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="B3" s="10" t="s">
@@ -758,16 +783,16 @@
         <v>34</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="O3" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>37</v>
@@ -778,27 +803,27 @@
       <c r="R3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="11"/>
+      <c r="S3" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="T3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="10" t="s">
         <v>41</v>
       </c>
+      <c r="U3" s="11"/>
       <c r="V3" s="10" t="s">
         <v>42</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="Y3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="Z3" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="AA3" s="10" t="s">
         <v>45</v>
@@ -812,36 +837,42 @@
       <c r="AD3" s="10" t="s">
         <v>48</v>
       </c>
+      <c r="AE3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF3" s="10" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.5" outlineLevel="0" r="4">
       <c r="A4" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="13" t="n">
+        <v>56</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="13" t="n">
         <v>1000</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="13" t="n">
+      <c r="J4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="13" t="n">
@@ -890,24 +921,30 @@
         <v>1</v>
       </c>
       <c r="Z4" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="AA4" s="14" t="n">
+      <c r="AC4" s="14" t="n">
         <v>200</v>
       </c>
-      <c r="AB4" s="13" t="n">
+      <c r="AD4" s="13" t="n">
         <v>300</v>
       </c>
-      <c r="AC4" s="13" t="n">
+      <c r="AE4" s="13" t="n">
         <v>400</v>
       </c>
-      <c r="AD4" s="13" t="n">
+      <c r="AF4" s="13" t="n">
         <v>500</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="1" r="5">
       <c r="A5" s="11" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -934,74 +971,82 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="15"/>
       <c r="Z5" s="15"/>
-      <c r="AA5" s="14"/>
+      <c r="AA5" s="15"/>
       <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
+      <c r="AC5" s="14"/>
       <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="1" r="6">
       <c r="A6" s="11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="P6" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
+      <c r="L6" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="1" r="7">
       <c r="A7" s="11" t="s">
@@ -1036,10 +1081,12 @@
       <c r="AB7" s="15"/>
       <c r="AC7" s="15"/>
       <c r="AD7" s="15"/>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="1" r="8">
       <c r="A8" s="11" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -1070,6 +1117,8 @@
       <c r="AB8" s="15"/>
       <c r="AC8" s="15"/>
       <c r="AD8" s="15"/>
+      <c r="AE8" s="15"/>
+      <c r="AF8" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="9"/>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.5" outlineLevel="0" r="10"/>
@@ -1079,13 +1128,13 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="14"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:M1"/>
-    <mergeCell ref="N1:Y1"/>
-    <mergeCell ref="Z1:AD2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:Y2"/>
+    <mergeCell ref="B1:H2"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:AA1"/>
+    <mergeCell ref="AB1:AF2"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:AA2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Export executives into outputExecutives.xlsx
</commit_message>
<xml_diff>
--- a/test/input/FullValuesAndComments.xlsx
+++ b/test/input/FullValuesAndComments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="4" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="5" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="DOC_SRC" sheetId="1" state="visible" r:id="rId2"/>
@@ -472,16 +472,16 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="AF3:AF8 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.556862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6117647058824"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5882352941176"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6509803921569"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -652,22 +652,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="G4" activeCellId="0" pane="topLeft" sqref="G4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="V1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="AF8" activeCellId="0" pane="topLeft" sqref="AF3:AF8"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.5921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.60392156862745"/>
     <col collapsed="false" hidden="false" max="8" min="4" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.4313725490196"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.9450980392157"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.4588235294118"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.4470588235294"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.956862745098"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.4705882352941"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.92941176470588"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.94117647058824"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.956862745098"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.3843137254902"/>
   </cols>
   <sheetData>
@@ -938,7 +938,7 @@
       <c r="AE4" s="13" t="n">
         <v>400</v>
       </c>
-      <c r="AF4" s="13" t="n">
+      <c r="AF4" s="0" t="n">
         <v>500</v>
       </c>
     </row>
@@ -976,7 +976,6 @@
       <c r="AC5" s="14"/>
       <c r="AD5" s="15"/>
       <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="1" r="6">
       <c r="A6" s="11" t="s">
@@ -1046,7 +1045,6 @@
       <c r="AC6" s="16"/>
       <c r="AD6" s="16"/>
       <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="1" r="7">
       <c r="A7" s="11" t="s">
@@ -1082,7 +1080,6 @@
       <c r="AC7" s="15"/>
       <c r="AD7" s="15"/>
       <c r="AE7" s="15"/>
-      <c r="AF7" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="1" r="8">
       <c r="A8" s="11" t="s">
@@ -1118,14 +1115,7 @@
       <c r="AC8" s="15"/>
       <c r="AD8" s="15"/>
       <c r="AE8" s="15"/>
-      <c r="AF8" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="1" r="9"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.5" outlineLevel="0" r="10"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="11"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="12"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="13"/>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="14"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B1:H2"/>

</xml_diff>